<commit_message>
Refactor attribute and mapping system; remove deprecated code
Reworked characteristic and knowledge classes to use new alias/code mapping via ATTRIBUTES, updating methods and internal structure. Removed deprecated mapping and package modules, and updated mapping modules to support new full code and alias handling. Added placeholder Location class. Updated Excel mapping integration and improved documentation and type usage throughout mapping code.
</commit_message>
<xml_diff>
--- a/game/mappings/T5Mappings.xlsx
+++ b/game/mappings/T5Mappings.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\Sophont\game\improvedmappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\Sophont\game\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AEC0AE-9AB6-4848-B0C1-4E2497AC1216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2E75259-4EE9-4608-9A2C-29821538F068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38520" yWindow="10335" windowWidth="16020" windowHeight="18180" firstSheet="1" activeTab="2" xr2:uid="{922B48FF-0A11-4648-9808-3CC4D7F2A9F4}"/>
+    <workbookView xWindow="38520" yWindow="10335" windowWidth="16020" windowHeight="18180" firstSheet="4" activeTab="5" xr2:uid="{922B48FF-0A11-4648-9808-3CC4D7F2A9F4}"/>
   </bookViews>
   <sheets>
     <sheet name="characteristics.master.en" sheetId="9" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="234">
   <si>
     <t>Code</t>
   </si>
@@ -767,6 +767,9 @@
   </si>
   <si>
     <t>Skill Code1</t>
+  </si>
+  <si>
+    <t>engineering</t>
   </si>
 </sst>
 </file>
@@ -4079,8 +4082,8 @@
   </sheetPr>
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6846,7 +6849,7 @@
   </sheetPr>
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -7862,8 +7865,8 @@
   </sheetPr>
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8166,7 +8169,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29</v>
       </c>
@@ -8174,7 +8177,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>30</v>
       </c>
@@ -8182,7 +8185,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>31</v>
       </c>
@@ -8190,7 +8193,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>32</v>
       </c>
@@ -8198,7 +8201,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>33</v>
       </c>
@@ -8206,7 +8209,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>34</v>
       </c>
@@ -8214,7 +8217,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>35</v>
       </c>
@@ -8222,7 +8225,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>36</v>
       </c>
@@ -8230,15 +8233,18 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>37</v>
       </c>
       <c r="B41" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>38</v>
       </c>
@@ -8246,7 +8252,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>39</v>
       </c>
@@ -8254,7 +8260,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>40</v>
       </c>
@@ -8262,7 +8268,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>41</v>
       </c>
@@ -8270,7 +8276,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>42</v>
       </c>
@@ -8278,7 +8284,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43</v>
       </c>
@@ -8286,7 +8292,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
Refactor GUID system and update related classes
Replaces UUID-based GUIDs with a custom 32-bit integer scheme using entity and owner namespaces. Updates all usages of GUIDs in game and GUI modules to use the new integer-based system, including Species, Genus, TreeOfLifeNode, Event, AttributePackage, Phene, and related code. Removes deprecated draggable GUI components and refactors UPP display logic for improved phene handling.
</commit_message>
<xml_diff>
--- a/game/mappings/T5Mappings.xlsx
+++ b/game/mappings/T5Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Python\Sophont\game\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2E75259-4EE9-4608-9A2C-29821538F068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B655BFD-50A7-4744-9B3D-CC77497C4089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38520" yWindow="10335" windowWidth="16020" windowHeight="18180" firstSheet="4" activeTab="5" xr2:uid="{922B48FF-0A11-4648-9808-3CC4D7F2A9F4}"/>
+    <workbookView xWindow="7500" yWindow="1380" windowWidth="16020" windowHeight="18180" firstSheet="1" activeTab="2" xr2:uid="{922B48FF-0A11-4648-9808-3CC4D7F2A9F4}"/>
   </bookViews>
   <sheets>
     <sheet name="characteristics.master.en" sheetId="9" r:id="rId1"/>
@@ -3289,7 +3289,7 @@
   <dimension ref="A1:G100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4082,8 +4082,8 @@
   </sheetPr>
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7865,7 +7865,7 @@
   </sheetPr>
   <dimension ref="A1:F90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>

</xml_diff>